<commit_message>
CAMBIOS PARA CORRECTA TOMA DE DATOS
</commit_message>
<xml_diff>
--- a/src/main/2023/BURGOS-ARANDA-SORIA/MEDICIONES PARTES/ARANDA-SORIA/APOYOS REALIZADOS BURGOS ARANDA SORIA 2023.xlsx
+++ b/src/main/2023/BURGOS-ARANDA-SORIA/MEDICIONES PARTES/ARANDA-SORIA/APOYOS REALIZADOS BURGOS ARANDA SORIA 2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\INES\Desktop\ROBERTO\src\main\2023\BURGOS-ARANDA-SORIA\MEDICIONES PARTES\ARANDA-SORIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271984AC-0C44-4637-AA10-67B3C6E3EF7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC5F65A-558D-4BFD-A70C-DEB1D57CB84D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30870" yWindow="3240" windowWidth="23580" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ARAUZO-CERVERA" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="86">
   <si>
     <t>APOYO</t>
   </si>
@@ -200,52 +200,94 @@
 </t>
   </si>
   <si>
-    <t>123-456 ARANDA-SINOVAS</t>
+    <t>12-56 ARANDA-SINOVAS</t>
+  </si>
+  <si>
+    <t>133.0</t>
   </si>
   <si>
     <t>NUEVO 1</t>
   </si>
   <si>
+    <t>1321.0</t>
+  </si>
+  <si>
     <t>NUEVO 2</t>
   </si>
   <si>
+    <t>321321.0</t>
+  </si>
+  <si>
     <t>NUEVO 3</t>
   </si>
   <si>
+    <t>3.21231321E8</t>
+  </si>
+  <si>
     <t>NUEVO 4</t>
   </si>
   <si>
+    <t>46.0</t>
+  </si>
+  <si>
     <t>NUEVO 5</t>
   </si>
   <si>
+    <t>456.0</t>
+  </si>
+  <si>
     <t>PAZ</t>
   </si>
   <si>
     <t>NUEVO 6</t>
   </si>
   <si>
+    <t>645644.0</t>
+  </si>
+  <si>
     <t>NUEVO 7</t>
   </si>
   <si>
+    <t>6.4654564E7</t>
+  </si>
+  <si>
     <t>NUEVO 8</t>
   </si>
   <si>
+    <t>65665.0</t>
+  </si>
+  <si>
     <t>NUEVO 9</t>
   </si>
   <si>
+    <t>8866.0</t>
+  </si>
+  <si>
     <t>NUEVO 10</t>
   </si>
   <si>
+    <t>663.0</t>
+  </si>
+  <si>
     <t>NUEVO 11</t>
   </si>
   <si>
+    <t>6664.0</t>
+  </si>
+  <si>
     <t>NUEVO 12</t>
   </si>
   <si>
+    <t>64987.0</t>
+  </si>
+  <si>
     <t>MIGUEL</t>
   </si>
   <si>
     <t>NUEVO 13</t>
+  </si>
+  <si>
+    <t>656646.0</t>
   </si>
   <si>
     <t>NUEVO 14</t>
@@ -2001,7 +2043,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>28</v>
       </c>
@@ -2030,7 +2072,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="285" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>28</v>
       </c>
@@ -2072,7 +2114,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="23.1015625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="6.8515625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="9.7109375" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="10.96875" customWidth="true" bestFit="true"/>
@@ -2138,8 +2180,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n" s="7">
-        <v>133.0</v>
+      <c r="A3" t="s" s="7">
+        <v>54</v>
       </c>
       <c r="B3" t="n" s="7">
         <v>0.0</v>
@@ -2178,12 +2220,12 @@
         <v>14</v>
       </c>
       <c r="N3" t="s" s="7">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n" s="7">
-        <v>1321.0</v>
+      <c r="A4" t="s" s="7">
+        <v>56</v>
       </c>
       <c r="B4" t="n" s="7">
         <v>0.0</v>
@@ -2222,12 +2264,12 @@
         <v>14</v>
       </c>
       <c r="N4" t="s" s="7">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n" s="7">
-        <v>321321.0</v>
+      <c r="A5" t="s" s="7">
+        <v>58</v>
       </c>
       <c r="B5" t="n" s="7">
         <v>34.0</v>
@@ -2266,12 +2308,12 @@
         <v>14</v>
       </c>
       <c r="N5" t="s" s="7">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n" s="7">
-        <v>3.21231321E8</v>
+      <c r="A6" t="s" s="7">
+        <v>60</v>
       </c>
       <c r="B6" t="n" s="7">
         <v>0.0</v>
@@ -2310,12 +2352,12 @@
         <v>14</v>
       </c>
       <c r="N6" t="s" s="7">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n" s="7">
-        <v>46.0</v>
+      <c r="A7" t="s" s="7">
+        <v>62</v>
       </c>
       <c r="B7" t="n" s="7">
         <v>0.0</v>
@@ -2354,12 +2396,12 @@
         <v>14</v>
       </c>
       <c r="N7" t="s" s="7">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n" s="7">
-        <v>456.0</v>
+      <c r="A8" t="s" s="7">
+        <v>64</v>
       </c>
       <c r="B8" t="n" s="7">
         <v>45.0</v>
@@ -2386,7 +2428,7 @@
         <v>45056.0</v>
       </c>
       <c r="J8" t="s" s="7">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="K8" t="s" s="7">
         <v>14</v>
@@ -2398,12 +2440,12 @@
         <v>14</v>
       </c>
       <c r="N8" t="s" s="7">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n" s="7">
-        <v>645644.0</v>
+      <c r="A9" t="s" s="7">
+        <v>67</v>
       </c>
       <c r="B9" t="n" s="7">
         <v>0.0</v>
@@ -2442,12 +2484,12 @@
         <v>14</v>
       </c>
       <c r="N9" t="s" s="7">
-        <v>61</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n" s="7">
-        <v>6.4654564E7</v>
+      <c r="A10" t="s" s="7">
+        <v>69</v>
       </c>
       <c r="B10" t="n" s="7">
         <v>0.0</v>
@@ -2486,12 +2528,12 @@
         <v>14</v>
       </c>
       <c r="N10" t="s" s="7">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n" s="7">
-        <v>65665.0</v>
+      <c r="A11" t="s" s="7">
+        <v>71</v>
       </c>
       <c r="B11" t="n" s="7">
         <v>4343.0</v>
@@ -2530,12 +2572,12 @@
         <v>14</v>
       </c>
       <c r="N11" t="s" s="7">
-        <v>63</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n" s="7">
-        <v>8866.0</v>
+      <c r="A12" t="s" s="7">
+        <v>73</v>
       </c>
       <c r="B12" t="n" s="7">
         <v>0.0</v>
@@ -2574,12 +2616,12 @@
         <v>14</v>
       </c>
       <c r="N12" t="s" s="7">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n" s="7">
-        <v>663.0</v>
+      <c r="A13" t="s" s="7">
+        <v>75</v>
       </c>
       <c r="B13" t="n" s="7">
         <v>0.0</v>
@@ -2618,12 +2660,12 @@
         <v>14</v>
       </c>
       <c r="N13" t="s" s="7">
-        <v>65</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n" s="7">
-        <v>6664.0</v>
+      <c r="A14" t="s" s="7">
+        <v>77</v>
       </c>
       <c r="B14" t="n" s="7">
         <v>0.0</v>
@@ -2662,12 +2704,12 @@
         <v>14</v>
       </c>
       <c r="N14" t="s" s="7">
-        <v>66</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n" s="7">
-        <v>64987.0</v>
+      <c r="A15" t="s" s="7">
+        <v>79</v>
       </c>
       <c r="B15" t="n" s="7">
         <v>0.0</v>
@@ -2694,7 +2736,7 @@
         <v>45066.0</v>
       </c>
       <c r="J15" t="s" s="7">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="K15" t="s" s="7">
         <v>14</v>
@@ -2706,12 +2748,12 @@
         <v>14</v>
       </c>
       <c r="N15" t="s" s="7">
-        <v>68</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n" s="7">
-        <v>656646.0</v>
+      <c r="A16" t="s" s="7">
+        <v>82</v>
       </c>
       <c r="B16" t="n" s="7">
         <v>0.0</v>
@@ -2750,7 +2792,7 @@
         <v>14</v>
       </c>
       <c r="N16" t="s" s="7">
-        <v>69</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18">
@@ -2779,7 +2821,7 @@
         <v>33.0</v>
       </c>
       <c r="K18" t="s" s="6">
-        <v>70</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19">
@@ -2808,7 +2850,7 @@
         <v>33.0</v>
       </c>
       <c r="K19" t="s" s="6">
-        <v>71</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>